<commit_message>
adaptions and adds links
</commit_message>
<xml_diff>
--- a/data/Mails.xlsx
+++ b/data/Mails.xlsx
@@ -5,13 +5,15 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Tabelle1!$A$1:$D$89</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Tabelle1!$A$1:$D$89</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Tabelle1!$A$1:$D$89</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -298,7 +300,7 @@
   <si>
     <t xml:space="preserve">Thema: Strom
 Frage/Mitteilung:
-Ich ziehe per 31 August nach Aarberg. Muss ich den Stromanschluss kündigen?
+Ich ziehe per 31 August nach Aarberg. Muss ich den Strom anschluss kündigen?
 </t>
   </si>
   <si>
@@ -419,7 +421,7 @@
   <si>
     <t xml:space="preserve">Thema: Sonstiges
 Frage/Mitteilung:
-Ist der Internetanschluss durch Sie auch außerhalb vom Kanton Bern, in 4613 Rickenbach nutzbar?
+Ist der Internet anschluss durch Sie auch außerhalb vom Kanton Bern, in 4613 Rickenbach nutzbar?
 </t>
   </si>
   <si>
@@ -802,7 +804,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Auszugsmeldung</t>
+    <t xml:space="preserve">Umzug : Auszugsmeldung</t>
   </si>
   <si>
     <t xml:space="preserve">Besten Dank für Ihre Mutationen.
@@ -851,7 +853,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Stromanmeldung</t>
+    <t xml:space="preserve">Strom anmeldung</t>
   </si>
   <si>
     <t xml:space="preserve">Sehr geehrte Damen und Herren
@@ -882,7 +884,7 @@
   <si>
     <t xml:space="preserve">Guten Nachmittag
 Die Familie Muster zieht aus.
-Bitte nehmen Sie per 30.9.2020 eine Zählerablesung vor.
+Bitte nehmen Sie per 30.9.2020 eine Zähler Ablesung vor.
 Besten Dank und freundliche Grüsse
 </t>
   </si>
@@ -895,7 +897,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Umzugsmeldung - Einzug</t>
+    <t xml:space="preserve">Umzug - Einzug</t>
   </si>
   <si>
     <t xml:space="preserve">Besten Dank und freundliche Grüsse</t>
@@ -1061,13 +1063,13 @@
     </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="*unknown*" xfId="20" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1137,21 +1139,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E89"/>
+  <dimension ref="A1:E83"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A80" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E84" activeCellId="0" sqref="E84"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A76" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B80" activeCellId="0" sqref="B80"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="63.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24.88"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.5255102040816"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="62.3673469387755"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.3010204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.3928571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1509,7 +1513,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="79.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="68.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
         <v>54</v>
       </c>
@@ -1763,7 +1767,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="79.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="68.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="3" t="s">
         <v>54</v>
       </c>
@@ -2322,7 +2326,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="92.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="3" t="s">
         <v>167</v>
       </c>
@@ -2391,30 +2395,6 @@
       <c r="E83" s="0" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="84" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="3"/>
-      <c r="B84" s="3"/>
-    </row>
-    <row r="85" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="3"/>
-      <c r="B85" s="3"/>
-    </row>
-    <row r="86" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="3"/>
-      <c r="B86" s="3"/>
-    </row>
-    <row r="87" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="3"/>
-      <c r="B87" s="3"/>
-    </row>
-    <row r="88" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="3"/>
-      <c r="B88" s="3"/>
-    </row>
-    <row r="89" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="3"/>
-      <c r="B89" s="3"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:D89"/>
@@ -2423,7 +2403,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>